<commit_message>
Working on edge conditions of low body fat and losses
</commit_message>
<xml_diff>
--- a/Calculators/Spreadsheet Calculators/MaxFatLoss.xlsx
+++ b/Calculators/Spreadsheet Calculators/MaxFatLoss.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="150" windowWidth="10800" windowHeight="4770"/>
+    <workbookView xWindow="240" yWindow="210" windowWidth="10800" windowHeight="4710"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -77,7 +77,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -120,7 +120,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -425,7 +425,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -453,7 +453,7 @@
         <v>12</v>
       </c>
       <c r="B2">
-        <v>8.1999999999999993</v>
+        <v>7.6</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
@@ -465,7 +465,7 @@
       </c>
       <c r="B3">
         <f>B1*B2/100</f>
-        <v>13.316799999999999</v>
+        <v>12.3424</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
@@ -475,7 +475,7 @@
       </c>
       <c r="F3" s="3">
         <f>E3*B3</f>
-        <v>319.60319999999996</v>
+        <v>296.2176</v>
       </c>
       <c r="G3" t="s">
         <v>11</v>
@@ -626,28 +626,28 @@
       </c>
       <c r="B14" s="3">
         <f>E14/D14</f>
-        <v>35.511466666666664</v>
+        <v>99.486933333333354</v>
       </c>
       <c r="D14">
         <v>9</v>
       </c>
       <c r="E14" s="3">
-        <f>IF(F3&gt;E13,E13,F3)</f>
-        <v>319.60319999999996</v>
+        <f>IF(F3&gt;E13,E13,E8-F3)</f>
+        <v>895.38240000000019</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E15">
         <f>E11+E12+E14</f>
-        <v>1089.2031999999999</v>
+        <v>1664.9824000000003</v>
       </c>
       <c r="F15" s="3">
         <f>E15-$B$4</f>
-        <v>-1120.7968000000001</v>
+        <v>-545.01759999999967</v>
       </c>
       <c r="G15" s="2">
         <f>F15/3500</f>
-        <v>-0.32022765714285717</v>
+        <v>-0.1557193142857142</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>